<commit_message>
New Definitions in Excel Download
</commit_message>
<xml_diff>
--- a/Titelblatt.xlsx
+++ b/Titelblatt.xlsx
@@ -88,9 +88,6 @@
     <t>Abfragetool MPE</t>
   </si>
   <si>
-    <t>Die Detaildaten der Mietpreiserhebung 2022 sind auf einem Abruftool verfügbar, das erreichbar ist unter: https://www.stadt-zuerich.ch/prd/de/index/statistik/themen/bauen-wohnen/mietpreise.html</t>
-  </si>
-  <si>
     <t>Platzhalter: Titel der Tabelle</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Anzahl Wohnungen in Sample 1 bzw. Sample 2</t>
   </si>
   <si>
-    <t>Samplegrösse für die betreffende Zelle pro Schicht 1 resp. Schicht 2: Anzahl Mietpreisinformationen, die vorliegen. Methodendokumentation unter: https://www.stadt-zuerich.ch/prd/de/index/statistik/themen/bauen-wohnen/mietpreise.html</t>
-  </si>
-  <si>
     <t>Grundgesamtheit für die betreffende Zelle: Gesamtzahl der Wohnungen der betreffenden Kategorie (Ausprägung von Raumeinheit, Gliederung, Zimmerzahl und Art der Gemeinnützigkeit).</t>
   </si>
   <si>
@@ -122,6 +116,12 @@
   </si>
   <si>
     <t>Die geschätzten Preise sind mit 95-%-Konfidenzintervallen unterlegt. Diese bezeichnen den Bereich, der bei unendlicher Wiederholung eines Zufallsexperiments mit einer Wahrscheinlichkeit von 95 Prozent den wahren Wert der Grundgesamtheit einschliesst. In der MPE liegen die 95-%-Konfidenzintervalle gesamtstädtisch ungefähr bei 4 Prozent der ausgewiesenen Medianpreise und Mittelwerte (absolute Breite des Konfidenzintervalls geteilt durch Schätzwert). Bei kleineren Raumeinheiten (z.B. Quartiere) sind die Unsicherheiten höher; die Konfidenzintervalle der ausgewiesenen Werte liegen im Bereich von 4 bis 8 Prozent und können unter Umständen bis gegen 20 Prozent steigen.</t>
+  </si>
+  <si>
+    <t>Samplegrösse für die betreffende Zelle pro Schicht 1 resp. Schicht 2: Anzahl Mietpreisinformationen, die vorliegen.</t>
+  </si>
+  <si>
+    <t>Die Detaildaten der Mietpreiserhebung 2022 sind auf einem Abruftool verfügbar, das erreichbar ist unter: https://www.stadt-zuerich.ch/prd/de/index/statistik/publikationen-angebote/datenbanken-anwendungen/mietpreiserhebung.html</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -561,7 +561,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -597,18 +597,18 @@
     </row>
     <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -616,7 +616,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -624,23 +624,23 @@
         <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -648,7 +648,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>